<commit_message>
fixed issues encountered during testing
</commit_message>
<xml_diff>
--- a/files/template.xlsx
+++ b/files/template.xlsx
@@ -60,9 +60,6 @@
     <t>PointOfContactName</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>HowTocite</t>
   </si>
   <si>
@@ -271,6 +268,9 @@
   </si>
   <si>
     <t>POCPhoneNumber</t>
+  </si>
+  <si>
+    <t>POCEmail</t>
   </si>
 </sst>
 </file>
@@ -615,7 +615,7 @@
   <dimension ref="A1:N201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +631,7 @@
     <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
     <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -641,10 +641,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
         <v>63</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -671,21 +671,21 @@
         <v>8</v>
       </c>
       <c r="L1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" t="s">
         <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <f>IFERROR(VLOOKUP(B2,CountryTable[],2,0),"")</f>
@@ -701,28 +701,28 @@
         <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I2">
         <v>344</v>
       </c>
       <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s">
         <v>72</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>73</v>
-      </c>
-      <c r="L2" t="s">
-        <v>74</v>
       </c>
       <c r="M2">
         <v>1123343444</v>
       </c>
       <c r="N2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -2021,15 +2021,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -2045,7 +2045,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -2053,7 +2053,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -2061,7 +2061,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -2069,7 +2069,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -2077,7 +2077,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -2085,7 +2085,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -2093,7 +2093,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -2101,7 +2101,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -2109,7 +2109,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -2117,7 +2117,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -2125,7 +2125,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -2141,7 +2141,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -2149,7 +2149,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>17</v>
@@ -2157,7 +2157,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18">
         <v>18</v>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19">
         <v>19</v>
@@ -2173,7 +2173,7 @@
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20">
         <v>20</v>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21">
         <v>21</v>
@@ -2189,7 +2189,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22">
         <v>22</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23">
         <v>23</v>
@@ -2205,7 +2205,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24">
         <v>24</v>
@@ -2213,7 +2213,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25">
         <v>25</v>
@@ -2221,7 +2221,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26">
         <v>26</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27">
         <v>27</v>
@@ -2237,7 +2237,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28">
         <v>28</v>
@@ -2245,7 +2245,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29">
         <v>29</v>
@@ -2253,7 +2253,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30">
         <v>30</v>
@@ -2261,7 +2261,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31">
         <v>31</v>
@@ -2269,7 +2269,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32">
         <v>32</v>
@@ -2277,7 +2277,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33">
         <v>33</v>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34">
         <v>34</v>
@@ -2293,7 +2293,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35">
         <v>35</v>
@@ -2301,7 +2301,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36">
         <v>36</v>
@@ -2309,7 +2309,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37">
         <v>37</v>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38">
         <v>38</v>
@@ -2325,7 +2325,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B39">
         <v>39</v>
@@ -2333,7 +2333,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40">
         <v>40</v>
@@ -2341,7 +2341,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41">
         <v>41</v>
@@ -2349,7 +2349,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B42">
         <v>42</v>
@@ -2357,7 +2357,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B43">
         <v>43</v>
@@ -2365,7 +2365,7 @@
     </row>
     <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B44">
         <v>44</v>
@@ -2373,7 +2373,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45">
         <v>46</v>
@@ -2381,7 +2381,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46">
         <v>47</v>
@@ -2389,7 +2389,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B47">
         <v>48</v>
@@ -2397,7 +2397,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B48">
         <v>49</v>
@@ -2405,7 +2405,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B49">
         <v>50</v>
@@ -2413,7 +2413,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B50">
         <v>51</v>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B51">
         <v>52</v>
@@ -2429,7 +2429,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B52">
         <v>53</v>
@@ -2437,7 +2437,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B53">
         <v>54</v>
@@ -2445,7 +2445,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B54">
         <v>55</v>
@@ -2453,7 +2453,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B55">
         <v>16</v>
@@ -2461,7 +2461,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B56">
         <v>45</v>
@@ -2495,17 +2495,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new field extent
</commit_message>
<xml_diff>
--- a/files/template.xlsx
+++ b/files/template.xlsx
@@ -15,10 +15,13 @@
     <sheet name="template" sheetId="1" r:id="rId1"/>
     <sheet name="countriestab" sheetId="2" r:id="rId2"/>
     <sheet name="statuses" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="countries">CountryTable[Column1]</definedName>
     <definedName name="CountryList">countriestab!$A$2:$A$53</definedName>
+    <definedName name="e">Sheet1!$A$1:$A$2</definedName>
+    <definedName name="ExtentTable">Sheet1!$A$1:$A$2</definedName>
     <definedName name="StatusList">statuses!$A$1:$A$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="83">
   <si>
     <t>Title</t>
   </si>
@@ -271,6 +274,15 @@
   </si>
   <si>
     <t>POCEmail</t>
+  </si>
+  <si>
+    <t>Extent</t>
+  </si>
+  <si>
+    <t>Full Country</t>
+  </si>
+  <si>
+    <t>Country Subset</t>
   </si>
 </sst>
 </file>
@@ -612,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N201"/>
+  <dimension ref="A1:O201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,16 +639,17 @@
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -659,28 +672,31 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>79</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>78</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -704,448 +720,451 @@
         <v>70</v>
       </c>
       <c r="H2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" t="s">
         <v>65</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>344</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>71</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>72</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>73</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>1123343444</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C3" t="str">
         <f>IFERROR(VLOOKUP(B3,CountryTable[],2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C4" t="str">
         <f>IFERROR(VLOOKUP(B4,CountryTable[],2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C5" t="str">
         <f>IFERROR(VLOOKUP(B5,CountryTable[],2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C6" t="str">
         <f>IFERROR(VLOOKUP(B6,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7" t="str">
         <f>IFERROR(VLOOKUP(B7,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8" t="str">
         <f>IFERROR(VLOOKUP(B8,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9" t="str">
         <f>IFERROR(VLOOKUP(B9,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C10" t="str">
         <f>IFERROR(VLOOKUP(B10,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11" t="str">
         <f>IFERROR(VLOOKUP(B11,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12" t="str">
         <f>IFERROR(VLOOKUP(B12,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13" t="str">
         <f>IFERROR(VLOOKUP(B13,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C14" t="str">
         <f>IFERROR(VLOOKUP(B14,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15" t="str">
         <f>IFERROR(VLOOKUP(B15,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16" t="str">
         <f>IFERROR(VLOOKUP(B16,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C17" t="str">
         <f>IFERROR(VLOOKUP(B17,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18" t="str">
         <f>IFERROR(VLOOKUP(B18,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C19" t="str">
         <f>IFERROR(VLOOKUP(B19,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C20" t="str">
         <f>IFERROR(VLOOKUP(B20,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C21" t="str">
         <f>IFERROR(VLOOKUP(B21,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C22" t="str">
         <f>IFERROR(VLOOKUP(B22,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C23" t="str">
         <f>IFERROR(VLOOKUP(B23,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C24" t="str">
         <f>IFERROR(VLOOKUP(B24,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C25" t="str">
         <f>IFERROR(VLOOKUP(B25,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C26" t="str">
         <f>IFERROR(VLOOKUP(B26,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C27" t="str">
         <f>IFERROR(VLOOKUP(B27,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M27" s="1"/>
-    </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C28" t="str">
         <f>IFERROR(VLOOKUP(B28,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M28" s="1"/>
-    </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="1"/>
+    </row>
+    <row r="29" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C29" t="str">
         <f>IFERROR(VLOOKUP(B29,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N29" s="1"/>
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C30" t="str">
         <f>IFERROR(VLOOKUP(B30,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M30" s="1"/>
-    </row>
-    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N30" s="1"/>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C31" t="str">
         <f>IFERROR(VLOOKUP(B31,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M31" s="1"/>
-    </row>
-    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N31" s="1"/>
+    </row>
+    <row r="32" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C32" t="str">
         <f>IFERROR(VLOOKUP(B32,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M32" s="1"/>
-    </row>
-    <row r="33" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C33" t="str">
         <f>IFERROR(VLOOKUP(B33,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M33" s="1"/>
-    </row>
-    <row r="34" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C34" t="str">
         <f>IFERROR(VLOOKUP(B34,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M34" s="1"/>
-    </row>
-    <row r="35" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N34" s="1"/>
+    </row>
+    <row r="35" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C35" t="str">
         <f>IFERROR(VLOOKUP(B35,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M35" s="1"/>
-    </row>
-    <row r="36" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N35" s="1"/>
+    </row>
+    <row r="36" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C36" t="str">
         <f>IFERROR(VLOOKUP(B36,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M36" s="1"/>
-    </row>
-    <row r="37" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N36" s="1"/>
+    </row>
+    <row r="37" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C37" t="str">
         <f>IFERROR(VLOOKUP(B37,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M37" s="1"/>
-    </row>
-    <row r="38" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N37" s="1"/>
+    </row>
+    <row r="38" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C38" t="str">
         <f>IFERROR(VLOOKUP(B38,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M38" s="1"/>
-    </row>
-    <row r="39" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N38" s="1"/>
+    </row>
+    <row r="39" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C39" t="str">
         <f>IFERROR(VLOOKUP(B39,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M39" s="1"/>
-    </row>
-    <row r="40" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N39" s="1"/>
+    </row>
+    <row r="40" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C40" t="str">
         <f>IFERROR(VLOOKUP(B40,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M40" s="1"/>
-    </row>
-    <row r="41" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N40" s="1"/>
+    </row>
+    <row r="41" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C41" t="str">
         <f>IFERROR(VLOOKUP(B41,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M41" s="1"/>
-    </row>
-    <row r="42" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N41" s="1"/>
+    </row>
+    <row r="42" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C42" t="str">
         <f>IFERROR(VLOOKUP(B42,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M42" s="1"/>
-    </row>
-    <row r="43" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N42" s="1"/>
+    </row>
+    <row r="43" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C43" t="str">
         <f>IFERROR(VLOOKUP(B43,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M43" s="1"/>
-    </row>
-    <row r="44" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N43" s="1"/>
+    </row>
+    <row r="44" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C44" t="str">
         <f>IFERROR(VLOOKUP(B44,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M44" s="1"/>
-    </row>
-    <row r="45" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N44" s="1"/>
+    </row>
+    <row r="45" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C45" t="str">
         <f>IFERROR(VLOOKUP(B45,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M45" s="1"/>
-    </row>
-    <row r="46" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N45" s="1"/>
+    </row>
+    <row r="46" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C46" t="str">
         <f>IFERROR(VLOOKUP(B46,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M46" s="1"/>
-    </row>
-    <row r="47" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N46" s="1"/>
+    </row>
+    <row r="47" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C47" t="str">
         <f>IFERROR(VLOOKUP(B47,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M47" s="1"/>
-    </row>
-    <row r="48" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N47" s="1"/>
+    </row>
+    <row r="48" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C48" t="str">
         <f>IFERROR(VLOOKUP(B48,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M48" s="1"/>
-    </row>
-    <row r="49" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N48" s="1"/>
+    </row>
+    <row r="49" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C49" t="str">
         <f>IFERROR(VLOOKUP(B49,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M49" s="1"/>
-    </row>
-    <row r="50" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N49" s="1"/>
+    </row>
+    <row r="50" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C50" t="str">
         <f>IFERROR(VLOOKUP(B50,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M50" s="1"/>
-    </row>
-    <row r="51" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N50" s="1"/>
+    </row>
+    <row r="51" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C51" t="str">
         <f>IFERROR(VLOOKUP(B51,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M51" s="1"/>
-    </row>
-    <row r="52" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N51" s="1"/>
+    </row>
+    <row r="52" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C52" t="str">
         <f>IFERROR(VLOOKUP(B52,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M52" s="1"/>
-    </row>
-    <row r="53" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N52" s="1"/>
+    </row>
+    <row r="53" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C53" t="str">
         <f>IFERROR(VLOOKUP(B53,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M53" s="1"/>
-    </row>
-    <row r="54" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N53" s="1"/>
+    </row>
+    <row r="54" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C54" t="str">
         <f>IFERROR(VLOOKUP(B54,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M54" s="1"/>
-    </row>
-    <row r="55" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N54" s="1"/>
+    </row>
+    <row r="55" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C55" t="str">
         <f>IFERROR(VLOOKUP(B55,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M55" s="1"/>
-    </row>
-    <row r="56" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N55" s="1"/>
+    </row>
+    <row r="56" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C56" t="str">
         <f>IFERROR(VLOOKUP(B56,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M56" s="1"/>
-    </row>
-    <row r="57" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N56" s="1"/>
+    </row>
+    <row r="57" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C57" t="str">
         <f>IFERROR(VLOOKUP(B57,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M57" s="1"/>
-    </row>
-    <row r="58" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N57" s="1"/>
+    </row>
+    <row r="58" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C58" t="str">
         <f>IFERROR(VLOOKUP(B58,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M58" s="1"/>
-    </row>
-    <row r="59" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N58" s="1"/>
+    </row>
+    <row r="59" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C59" t="str">
         <f>IFERROR(VLOOKUP(B59,CountryTable[],2,0),"")</f>
         <v/>
       </c>
-      <c r="M59" s="1"/>
-    </row>
-    <row r="60" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N59" s="1"/>
+    </row>
+    <row r="60" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C60" t="str">
         <f>IFERROR(VLOOKUP(B60,CountryTable[],2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="61" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C61" t="str">
         <f>IFERROR(VLOOKUP(B61,CountryTable[],2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C62" t="str">
         <f>IFERROR(VLOOKUP(B62,CountryTable[],2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="63" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C63" t="str">
         <f>IFERROR(VLOOKUP(B63,CountryTable[],2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="64" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C64" t="str">
         <f>IFERROR(VLOOKUP(B64,CountryTable[],2,0),"")</f>
         <v/>
@@ -1974,18 +1993,24 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error in country name" error="Please select a country from dropdown" promptTitle="Countries" prompt="Please select a country" sqref="B213">
       <formula1>"countries!$A$1:$A$54"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B212">
       <formula1>CountryList</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error in status" error="Please select a status from dropdown" promptTitle="Status" prompt="Please select a status " sqref="H2:H205">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error in status" error="Please select a status from dropdown" promptTitle="Status" prompt="Please select a status " sqref="I2:I205">
       <formula1>StatusList</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Error in country name" error="Please select a country from drop down" promptTitle="Country" prompt="Please select a country" sqref="B2">
       <formula1>countries</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Select Extent" promptTitle="Please select Extent" sqref="H2">
+      <formula1>ExtentTable</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H201">
+      <formula1>ExtentTable</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1997,7 +2022,7 @@
           <x14:formula1>
             <xm:f>countriestab!$A$2:$A$53</xm:f>
           </x14:formula1>
-          <xm:sqref>L60</xm:sqref>
+          <xm:sqref>M60</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2511,4 +2536,32 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>